<commit_message>
added matrix of other weather generators
</commit_message>
<xml_diff>
--- a/write_ups/02_european_heatwave_paper/words/comparison_of_other_weather_engines/weather engine comparison.xlsx
+++ b/write_ups/02_european_heatwave_paper/words/comparison_of_other_weather_engines/weather engine comparison.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -117,13 +118,100 @@
   </si>
   <si>
     <t>CHECK LEFT FOR LINKS TO ABOVE IN TABLE 1</t>
+  </si>
+  <si>
+    <t>IMAGE</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>CLIMGEN</t>
+  </si>
+  <si>
+    <t>Time scale</t>
+  </si>
+  <si>
+    <t>Bi-weekly</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Precipitation occurrence</t>
+  </si>
+  <si>
+    <t>Precipitation amount</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Transition probabilities of a first-order, two-state Markov chain (two parameters)</t>
+  </si>
+  <si>
+    <t>Transition probabilities of a second-order, two-state Markov chain (two parameters)</t>
+  </si>
+  <si>
+    <t>Same procedure as WGEN, but parameters are computed at the monthly scale</t>
+  </si>
+  <si>
+    <t>Trasition probabilities of a third-order, two-state Markov chain (eight parameters)</t>
+  </si>
+  <si>
+    <t>Lengths of alternate dry and wet sequences chosen from a semi-empirical distribution fitted to the observed series (21 parameters)</t>
+  </si>
+  <si>
+    <t>Gamma distribution (two parameters)</t>
+  </si>
+  <si>
+    <t>Weibull distribution (two parameters)</t>
+  </si>
+  <si>
+    <t>Skewed normal distribution (three parameters)</t>
+  </si>
+  <si>
+    <t>Mixed exponential distribution (three parameters)</t>
+  </si>
+  <si>
+    <t>Semi-empirical distribution (21 parameters)</t>
+  </si>
+  <si>
+    <t>Latent Gaussian, Observed data reduced to time series of residuals. First-order autoregressive model to generate new ones</t>
+  </si>
+  <si>
+    <t>(Also huss and ps) Latent Gaussian with temporal behaviour governed by auto-regressive model whose rediausl and parameters are correlated throught resampling of principle component time series of empirical orthogonal function modes</t>
+  </si>
+  <si>
+    <t>Same as WGEN</t>
+  </si>
+  <si>
+    <t>Latent Gaussian, using parameters from each month, random numbers to generate the SD, second random number used as random number used as first for next day</t>
+  </si>
+  <si>
+    <t>Same as WGEN, apart from pre-set cross-correlation between reisduals</t>
+  </si>
+  <si>
+    <t>A-WGEN-2D</t>
+  </si>
+  <si>
+    <t>WXGEN</t>
+  </si>
+  <si>
+    <t>Met&amp;Roll</t>
+  </si>
+  <si>
+    <t>AAFC-WG</t>
+  </si>
+  <si>
+    <t>UKCP09</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -139,6 +227,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -148,7 +257,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -156,11 +265,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -168,6 +292,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -448,14 +583,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.83203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="43.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.1640625" style="3" bestFit="1" customWidth="1"/>
@@ -463,7 +598,7 @@
     <col min="7" max="7" width="41.33203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -506,7 +641,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -565,7 +700,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -607,4 +742,193 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="A1:E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="30.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="24" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="28" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="42" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C7:E7"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
extracting values from clagarmi script
</commit_message>
<xml_diff>
--- a/write_ups/02_european_heatwave_paper/words/comparison_of_other_weather_engines/weather engine comparison.xlsx
+++ b/write_ups/02_european_heatwave_paper/words/comparison_of_other_weather_engines/weather engine comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmiparks/git/IMAGE/write_ups/02_european_heatwave_paper/words/comparison_of_other_weather_engines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7B4C2F-48AE-314A-AFE7-998968DACCEC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB983BB-965E-924A-9DA0-7829A51FA546}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1000" yWindow="-24060" windowWidth="38440" windowHeight="24040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-17780" windowWidth="32000" windowHeight="23540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weather Engines" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="68">
   <si>
     <t>WeaGETS</t>
   </si>
@@ -66,15 +66,9 @@
     <t>Transition probabilities of a second-order, two-state Markov chain (two parameters)</t>
   </si>
   <si>
-    <t>Same procedure as WGEN, but parameters are computed at the monthly scale</t>
-  </si>
-  <si>
     <t>Trasition probabilities of a third-order, two-state Markov chain (eight parameters)</t>
   </si>
   <si>
-    <t>Lengths of alternate dry and wet sequences chosen from a semi-empirical distribution fitted to the observed series (21 parameters)</t>
-  </si>
-  <si>
     <t>Gamma distribution (two parameters)</t>
   </si>
   <si>
@@ -87,18 +81,9 @@
     <t>Mixed exponential distribution (three parameters)</t>
   </si>
   <si>
-    <t>Semi-empirical distribution (21 parameters)</t>
-  </si>
-  <si>
     <t>Latent Gaussian, Observed data reduced to time series of residuals. First-order autoregressive model to generate new ones</t>
   </si>
   <si>
-    <t>(Also huss and ps) Latent Gaussian with temporal behaviour governed by auto-regressive model whose rediausl and parameters are correlated throught resampling of principle component time series of empirical orthogonal function modes</t>
-  </si>
-  <si>
-    <t>Same as WGEN</t>
-  </si>
-  <si>
     <t>Latent Gaussian, using parameters from each month, random numbers to generate the SD, second random number used as random number used as first for next day</t>
   </si>
   <si>
@@ -108,9 +93,6 @@
     <t>A-WGEN-2D</t>
   </si>
   <si>
-    <t>WXGEN</t>
-  </si>
-  <si>
     <t>Met&amp;Roll</t>
   </si>
   <si>
@@ -165,15 +147,9 @@
     <t>LARS-WG</t>
   </si>
   <si>
-    <t>Built for Canada</t>
-  </si>
-  <si>
     <t>First published</t>
   </si>
   <si>
-    <t>Matlab-based with correction post-processing of variables</t>
-  </si>
-  <si>
     <t>Multisite</t>
   </si>
   <si>
@@ -201,9 +177,6 @@
     <t>Seasonal</t>
   </si>
   <si>
-    <t>UK only</t>
-  </si>
-  <si>
     <t>Hybrid of stochastic-statistical and physical-dynamical</t>
   </si>
   <si>
@@ -216,13 +189,49 @@
     <t>String of beads model</t>
   </si>
   <si>
-    <t>Something to do with how many cloud squares have been activated (string of beads model?)</t>
-  </si>
-  <si>
     <t>Generated from modular system, mix of deterministic and stochastic elements</t>
   </si>
   <si>
     <t>Spline interpolation procedure from monthly means and standard deviations</t>
+  </si>
+  <si>
+    <t>Latent Gaussian, Observed data reduced to time series of residuals. First-order autoregressive model to generate new ones. Influenced by whether wet or dry day before</t>
+  </si>
+  <si>
+    <t>(Also huss and ps) Latent Gaussian with temporal behaviour governed by auto-regressive model whose residuals and parameters are correlated throught resampling of principle component time series of empirical orthogonal function modes</t>
+  </si>
+  <si>
+    <t>Example simulated daily tempearture, number of solar hours, precipitation</t>
+  </si>
+  <si>
+    <t>Lengths of alternate dry and wet sequences chosen from a semi-empirical distribution fitted to the observed series approximated by a Fourier series (21 parameters)</t>
+  </si>
+  <si>
+    <t>Semi-empirical distribution approximated by a Fourier series (21 parameters)</t>
+  </si>
+  <si>
+    <t>WXGEN (EPIC)</t>
+  </si>
+  <si>
+    <t>Built for Canada and temperature, solar precipitation</t>
+  </si>
+  <si>
+    <t>Censored gamma distribution (two parameters)</t>
+  </si>
+  <si>
+    <t>Built for Canadafor precipitation, temperature, solar radiation, wind speed and relative humidity</t>
+  </si>
+  <si>
+    <t>UK only for temperature, rainfall, humidity and sunshine</t>
+  </si>
+  <si>
+    <t>Something to do with how many cloud squares have been activated (Neyman-Scott Rectangular Pulses)</t>
+  </si>
+  <si>
+    <t>Matlab-based with correction post-processing of variables of preciptation and maximum and minimum temperature</t>
+  </si>
+  <si>
+    <t>Can be any input variable</t>
   </si>
 </sst>
 </file>
@@ -321,11 +330,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -609,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -630,22 +639,22 @@
         <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>7</v>
@@ -657,445 +666,449 @@
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C2" s="4">
         <v>1984</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C3" s="4">
         <v>1990</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C4" s="4">
         <v>1991</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="4"/>
+      <c r="K4" s="4" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C5" s="4">
         <v>1994</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C6" s="4">
         <v>1995</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C7" s="4">
         <v>2000</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C8" s="4">
         <v>2000</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C9" s="4">
         <v>2001</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C10" s="4">
         <v>2003</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C11" s="4">
         <v>2004</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="J11" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C12" s="4">
         <v>2009</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C13" s="4">
         <v>2012</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C14" s="4">
         <v>2017</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="K14" s="4"/>
     </row>
@@ -1104,29 +1117,31 @@
         <v>2</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C15" s="4">
         <v>2017</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>